<commit_message>
Source and include directories. Consistent code formatting. Updated TODO and Readme files.
</commit_message>
<xml_diff>
--- a/Training Times.xlsx
+++ b/Training Times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Octopus\Documents\Git\TicTacToeMachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DC4F31-71FD-404A-8B44-B0E1577E4818}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27F35A3-5C34-4961-90C6-B687E2E11B89}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{BF7A4B15-07AC-4DE8-8122-179B39B8A1AB}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Population</t>
-  </si>
-  <si>
-    <t>Iterations</t>
   </si>
   <si>
     <t>All with 1 hidden layer with 1 hidden unit</t>
@@ -38,12 +35,21 @@
   <si>
     <t>Before Optimizations</t>
   </si>
+  <si>
+    <t>After Optimizations</t>
+  </si>
+  <si>
+    <t>Percent Of Original Time</t>
+  </si>
+  <si>
+    <t>Avg.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +60,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -89,10 +102,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -105,9 +119,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -419,250 +450,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D13B31-3E86-48A8-9FE9-22E380DBC8B6}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" customWidth="1"/>
-    <col min="4" max="4" width="3" customWidth="1"/>
-    <col min="5" max="6" width="3.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="4" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" customWidth="1"/>
+    <col min="15" max="15" width="3" customWidth="1"/>
+    <col min="16" max="17" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="5">
+        <v>100</v>
       </c>
       <c r="C3" s="5">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5">
-        <v>40</v>
-      </c>
-      <c r="E3" s="5">
-        <v>60</v>
-      </c>
-      <c r="F3" s="5">
-        <v>80</v>
-      </c>
-      <c r="G3" s="5">
+        <v>200</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="5">
         <v>100</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="5">
+        <v>100</v>
+      </c>
+      <c r="N3" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>20</v>
-      </c>
-      <c r="B5" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8</v>
+      </c>
       <c r="C5" s="3">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5">
+        <v>40</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5</v>
+      </c>
+      <c r="K5" s="5">
+        <v>40</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="10">
+        <f>H5/B5</f>
+        <v>0.375</v>
+      </c>
+      <c r="N5" s="10">
+        <f>I5/C5</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3">
+        <v>34</v>
+      </c>
+      <c r="F6" s="5">
+        <v>60</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4">
+        <v>13</v>
+      </c>
+      <c r="K6" s="5">
+        <v>60</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="10">
+        <f>H6/B6</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="N6" s="10">
+        <f>I6/C6</f>
+        <v>0.38235294117647056</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3">
+        <v>62</v>
+      </c>
+      <c r="F7" s="5">
+        <v>80</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4">
+        <v>12</v>
+      </c>
+      <c r="I7" s="4">
+        <v>24</v>
+      </c>
+      <c r="K7" s="5">
+        <v>80</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="10">
+        <f>H7/B7</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="N7" s="10">
+        <f>I7/C7</f>
+        <v>0.38709677419354838</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>100</v>
+      </c>
+      <c r="B8" s="3">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3">
+        <v>84</v>
+      </c>
+      <c r="F8" s="5">
+        <v>100</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4">
+        <v>17</v>
+      </c>
+      <c r="I8" s="4">
+        <v>37</v>
+      </c>
+      <c r="K8" s="5">
+        <v>100</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="10">
+        <f t="shared" ref="M6:N10" si="0">H8/B8</f>
+        <v>0.36956521739130432</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.44047619047619047</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>200</v>
+      </c>
+      <c r="B9" s="3">
+        <v>148</v>
+      </c>
+      <c r="C9" s="3">
+        <v>376</v>
+      </c>
+      <c r="F9" s="5">
+        <v>200</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4">
+        <v>68</v>
+      </c>
+      <c r="I9" s="4">
+        <v>122</v>
+      </c>
+      <c r="K9" s="5">
+        <v>200</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.45945945945945948</v>
+      </c>
+      <c r="N9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.32446808510638298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>500</v>
+      </c>
+      <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="D5" s="3">
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>500</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4">
+        <v>260</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>500</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="10" t="e">
+        <f>H10/B10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="11">
+        <f>AVERAGE(M5:N9)</f>
+        <v>0.3868378985263673</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>40</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3">
-        <v>4</v>
-      </c>
-      <c r="F6" s="3">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3">
-        <v>8</v>
-      </c>
-      <c r="H6" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>60</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3">
-        <v>13</v>
-      </c>
-      <c r="G7" s="3">
-        <v>18</v>
-      </c>
-      <c r="H7" s="3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>80</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3">
-        <v>23</v>
-      </c>
-      <c r="G8" s="3">
-        <v>28</v>
-      </c>
-      <c r="H8" s="3">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>100</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="3">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3">
-        <v>27</v>
-      </c>
-      <c r="F9" s="3">
-        <v>36</v>
-      </c>
-      <c r="G9" s="3">
-        <v>46</v>
-      </c>
-      <c r="H9" s="3">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>200</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="3">
-        <v>36</v>
-      </c>
-      <c r="D10" s="3">
-        <v>71</v>
-      </c>
-      <c r="E10" s="3">
-        <v>111</v>
-      </c>
-      <c r="F10" s="3">
-        <v>142</v>
-      </c>
-      <c r="G10" s="3">
-        <v>148</v>
-      </c>
-      <c r="H10" s="3">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:H2"/>
+  <mergeCells count="21">
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="F1:I2"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K1:N2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:H10">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="H5:I9 H10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:C10">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:I10">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
Inline, emplace_back(), and unaryEpr() optimizations.
</commit_message>
<xml_diff>
--- a/Training Times.xlsx
+++ b/Training Times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Octopus\Documents\Git\TicTacToeMachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27F35A3-5C34-4961-90C6-B687E2E11B89}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC2532A-CAF3-4758-8ED8-D254F1410113}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{BF7A4B15-07AC-4DE8-8122-179B39B8A1AB}"/>
   </bookViews>
@@ -116,12 +116,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -135,6 +129,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D13B31-3E86-48A8-9FE9-22E380DBC8B6}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,67 +472,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
       <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="5">
+      <c r="A3" s="7"/>
+      <c r="B3" s="10">
         <v>100</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="10">
         <v>200</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="5">
+      <c r="H3" s="10">
         <v>100</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="10">
         <v>200</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="5">
+      <c r="M3" s="10">
         <v>100</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="10">
         <v>200</v>
       </c>
     </row>
@@ -540,23 +540,23 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="K4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>40</v>
       </c>
       <c r="B5" s="3">
@@ -565,31 +565,31 @@
       <c r="C5" s="3">
         <v>16</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="10">
         <v>40</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="4">
         <v>3</v>
       </c>
       <c r="I5" s="4">
         <v>5</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="10">
         <v>40</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="10">
-        <f>H5/B5</f>
+      <c r="L5" s="10"/>
+      <c r="M5" s="8">
+        <f t="shared" ref="M5:N7" si="0">H5/B5</f>
         <v>0.375</v>
       </c>
-      <c r="N5" s="10">
-        <f>I5/C5</f>
+      <c r="N5" s="8">
+        <f t="shared" si="0"/>
         <v>0.3125</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>60</v>
       </c>
       <c r="B6" s="3">
@@ -598,31 +598,31 @@
       <c r="C6" s="3">
         <v>34</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="10">
         <v>60</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="4">
         <v>7</v>
       </c>
       <c r="I6" s="4">
         <v>13</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="10">
         <v>60</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="10">
-        <f>H6/B6</f>
+      <c r="L6" s="10"/>
+      <c r="M6" s="8">
+        <f t="shared" si="0"/>
         <v>0.3888888888888889</v>
       </c>
-      <c r="N6" s="10">
-        <f>I6/C6</f>
+      <c r="N6" s="8">
+        <f t="shared" si="0"/>
         <v>0.38235294117647056</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <v>80</v>
       </c>
       <c r="B7" s="3">
@@ -631,31 +631,31 @@
       <c r="C7" s="3">
         <v>62</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="10">
         <v>80</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="4">
         <v>12</v>
       </c>
       <c r="I7" s="4">
         <v>24</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="10">
         <v>80</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="10">
-        <f>H7/B7</f>
+      <c r="L7" s="10"/>
+      <c r="M7" s="8">
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="N7" s="10">
-        <f>I7/C7</f>
+      <c r="N7" s="8">
+        <f t="shared" si="0"/>
         <v>0.38709677419354838</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>100</v>
       </c>
       <c r="B8" s="3">
@@ -664,31 +664,31 @@
       <c r="C8" s="3">
         <v>84</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="10">
         <v>100</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="4">
         <v>17</v>
       </c>
       <c r="I8" s="4">
         <v>37</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="10">
         <v>100</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="10">
-        <f t="shared" ref="M6:N10" si="0">H8/B8</f>
+      <c r="L8" s="10"/>
+      <c r="M8" s="8">
+        <f t="shared" ref="M8:N10" si="1">H8/B8</f>
         <v>0.36956521739130432</v>
       </c>
-      <c r="N8" s="10">
-        <f t="shared" si="0"/>
+      <c r="N8" s="8">
+        <f t="shared" si="1"/>
         <v>0.44047619047619047</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>200</v>
       </c>
       <c r="B9" s="3">
@@ -697,31 +697,31 @@
       <c r="C9" s="3">
         <v>376</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="10">
         <v>200</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="4">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I9" s="4">
         <v>122</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="10">
         <v>200</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="10">
-        <f t="shared" si="0"/>
-        <v>0.45945945945945948</v>
-      </c>
-      <c r="N9" s="10">
-        <f t="shared" si="0"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.41216216216216217</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="1"/>
         <v>0.32446808510638298</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>500</v>
       </c>
       <c r="B10" s="4">
@@ -730,40 +730,40 @@
       <c r="C10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="10">
         <v>500</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="4">
         <v>260</v>
       </c>
       <c r="I10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="10">
         <v>500</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="10" t="e">
+      <c r="L10" s="10"/>
+      <c r="M10" s="8" t="e">
         <f>H10/B10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="10" t="e">
-        <f t="shared" si="0"/>
+      <c r="N10" s="8" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="9">
         <f>AVERAGE(M5:N9)</f>
-        <v>0.3868378985263673</v>
+        <v>0.38210816879663756</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -773,19 +773,16 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
+    <row r="24" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>67</v>
+      </c>
+      <c r="K24">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="F1:I2"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
@@ -794,8 +791,19 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="N3:N4"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="F1:I2"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:I9 H10">
     <cfRule type="colorScale" priority="5">

</xml_diff>